<commit_message>
+final results with tuning
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tarnebj1\Dropbox\1_School\JohnsHopkins\MachineLearning649\assignment6\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarney/Dropbox/1_School/JohnsHopkins/MachineLearning649/assignment6/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F33D2150-0DD0-FE42-9E80-11637FCD6D13}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34404" yWindow="2400" windowWidth="28656" windowHeight="24000"/>
+    <workbookView xWindow="34400" yWindow="2400" windowWidth="28660" windowHeight="24000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,54 +31,63 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>Data Sets</t>
-  </si>
-  <si>
-    <t>Classificaiton Accuracy (%)</t>
-  </si>
-  <si>
-    <t>5-fold Cross Validation Results</t>
-  </si>
-  <si>
-    <t>Breast Cancer</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="17">
   <si>
     <t>Glass</t>
   </si>
   <si>
-    <t>Iris</t>
-  </si>
-  <si>
     <t>Soybean</t>
   </si>
   <si>
-    <t>Vote</t>
-  </si>
-  <si>
-    <t>Momentum</t>
-  </si>
-  <si>
-    <t>Algorithm: FeedForwar Neural Network</t>
-  </si>
-  <si>
-    <t>1 hidden layer</t>
-  </si>
-  <si>
-    <t>2 hidden layers</t>
-  </si>
-  <si>
-    <t>0 hidden layer</t>
-  </si>
-  <si>
-    <t>2+ hidden layers</t>
+    <t>Data Set</t>
+  </si>
+  <si>
+    <t>Voting</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iris </t>
+  </si>
+  <si>
+    <t>#Classes</t>
+  </si>
+  <si>
+    <t>1 Layer (no hidden)</t>
+  </si>
+  <si>
+    <t>2 layers (1 hidden)</t>
+  </si>
+  <si>
+    <t>3 layers (2 hidden)</t>
+  </si>
+  <si>
+    <t>Data Set: Voting</t>
+  </si>
+  <si>
+    <t>number of nodes</t>
+  </si>
+  <si>
+    <t>Classification Accuracy (%)</t>
+  </si>
+  <si>
+    <t>learning rate</t>
+  </si>
+  <si>
+    <t>Best average  (across 5-fold) performance vs. learning rate</t>
+  </si>
+  <si>
+    <t>Best average  (across 5-fold) performance vs number of nodes</t>
+  </si>
+  <si>
+    <t>Best average (across 5-fold) performance vs. number of layers</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -119,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -128,149 +138,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -281,7 +152,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -298,43 +169,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,127 +504,335 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.69921875" customWidth="1"/>
-    <col min="3" max="4" width="13.796875" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="7" max="7" width="6.19921875" customWidth="1"/>
-    <col min="8" max="8" width="8.796875" customWidth="1"/>
+    <col min="7" max="7" width="6.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8.83203125" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
     <col min="10" max="10" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="B2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="13"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15"/>
-      <c r="B5" s="7" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="F5" s="13"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" ht="63" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="9">
+        <v>6</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6" s="10"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>4</v>
+      </c>
       <c r="F7" s="11"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="B11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="D11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9">
+        <v>3</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="9">
+        <v>6</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="12"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>4</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="12"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
-        <v>8</v>
-      </c>
+      <c r="D20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="9">
+        <v>2</v>
+      </c>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2</v>
+      </c>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="9">
+        <v>3</v>
+      </c>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="9">
+        <v>6</v>
+      </c>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>4</v>
+      </c>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+    </row>
+    <row r="35" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:F4"/>
+  <mergeCells count="3">
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>